<commit_message>
update 13 data augmentation
</commit_message>
<xml_diff>
--- a/data/patterns.xlsx
+++ b/data/patterns.xlsx
@@ -20,18 +20,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">for_the_plaintiff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">julgo procedente</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">Autor(a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome_variável</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expressão regular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felipe de Barros Lima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumidor Telecom Telas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ausência de prova.{,200}(telas?|registros?)\s*(sist[êe]mic[ao]|de sistema)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mÁRIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CondESC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cc]onden[o|a].{2,30}distrito federal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aor Suriz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indenizatória Improcedente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumidor.*inscrição devida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elenise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processos judiciais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\s\d{7}\-\d{2}\.\d{4}\.\d{1}\.\d{2}\.\d{4}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achar Lei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lei\s+[\d\.]{,6}/\w{2,4}</t>
   </si>
 </sst>
 </file>
@@ -106,9 +148,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -128,33 +174,89 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.84"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>